<commit_message>
osmanbo stage-2 add A7 to A20
</commit_message>
<xml_diff>
--- a/osmanbo/evidence.xlsx
+++ b/osmanbo/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osman\Desktop\gon_nft\osmanbo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A871A8-5FB8-4E50-9779-B60575C35235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9EA693-E3FA-4F37-9162-872B6D5B2555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10410" yWindow="735" windowWidth="23820" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3345" yWindow="630" windowWidth="31740" windowHeight="13155" firstSheet="2" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -39,12 +39,25 @@
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="86">
   <si>
     <t>TxHash</t>
   </si>
@@ -58,27 +71,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -167,13 +165,163 @@
   </si>
   <si>
     <t>949BDAD98EA14E07B31CC817E582C17BF2D15AD39D90065259E1ABE2507E4B2D</t>
+  </si>
+  <si>
+    <t>ibc/46D96CBDE13AE74C83DAE51E32F5122FA8BEE2E7776FE56CC66E717F445BFEBE</t>
+  </si>
+  <si>
+    <t>id8</t>
+  </si>
+  <si>
+    <t>ibc/675BD60A40CBAF78BBC555FCC36AEF0531C02F33A866F22D283AA9EC66F8E57A</t>
+  </si>
+  <si>
+    <t>id9</t>
+  </si>
+  <si>
+    <t>ibc/3E08D2CB258DF353131DE625F2993A129346CCDF30C6B55C4A8130CAD58D2FD7</t>
+  </si>
+  <si>
+    <t>id10</t>
+  </si>
+  <si>
+    <t>ibc/E64C825DC1126FA905F64E5B3121B4B9F95B7737A178F2BFF6961641C8EA91A5</t>
+  </si>
+  <si>
+    <t>id11</t>
+  </si>
+  <si>
+    <t>ibc/B0B58C9D23665A4012F47759108BFF4DE6759D3A3733A48A60D814B03A21C7CF</t>
+  </si>
+  <si>
+    <t>id12</t>
+  </si>
+  <si>
+    <t>ibc/FE6E4F2977390FD4EDDD56C9CEC03A9F754D07662E0567F76BB9FBE560C30861</t>
+  </si>
+  <si>
+    <t>id13</t>
+  </si>
+  <si>
+    <t>EC38C32DCD8DB0BCE2860942BB3A2A97997A9C0801F05250220D042E81D10DF0</t>
+  </si>
+  <si>
+    <t>670E1C9D456AB7EC20B86EFED2A75E3B77CEDB66E63125F9D833F4A0647A2EC1</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>67F138B2EA5BA8DECC329365CBB443EFB083319E9C709E13F4CDE92E794F9CF0</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>CBCCF0C2594B0B1A029E6AEC3A8B51EA4258D2A446E10F1225B1DA90F5CB6D37</t>
+  </si>
+  <si>
+    <t>1F3E987D0E8E5ACBE7B85A388C48D4F0E869B8B86E6A6FC44036CA1E067F3891</t>
+  </si>
+  <si>
+    <t>46849939873EE04C872856B24B9E9BA995EEDD114FE52BE6D5E452C85C17E0F0</t>
+  </si>
+  <si>
+    <t>2D24972BB7F35521B9AB0EB8383A6FFB156087BBEF73847BAA91BEBD253B0E06</t>
+  </si>
+  <si>
+    <t>2C7A1E83BC476F4E6D0FF9A3B81939324C64BD7B792E5935A50C86263FA71BF1</t>
+  </si>
+  <si>
+    <t>1F64ACBB9D9D3EE259BFA6E8A0412437FC69BFD73984BB60BEA9F4FC26166E37</t>
+  </si>
+  <si>
+    <t>CBD8457C0FDE8E9F2C6E83B805582431D7E0004F5A74131C78DE80F563ABA89D</t>
+  </si>
+  <si>
+    <t>8EE6BD2942CD0AACC6FA81A03C2A8A11F33BF3EE0777B61292DF4CF1997D9498</t>
+  </si>
+  <si>
+    <t>8F4582EC69F88142E98B2B72B9F5AB6159D03FB5B5793FF2C5E520E0FDCE3DDB</t>
+  </si>
+  <si>
+    <t>9BC0FE63EED6B1AF48CA5FCFF3E667C07561363198162712A11667D89D617AD9</t>
+  </si>
+  <si>
+    <t>F9728568C28B7DD502CD792C198A1CB9027A1B69F028A7B5750F1CF47BD3BE8A</t>
+  </si>
+  <si>
+    <t>603AAF1F655C371D365381E6D1F1E1339B0F6C8BB26A63D7CC44FFBBA7BAD5EB</t>
+  </si>
+  <si>
+    <t>82A9621DE4D2732FE7ACED1FCB0DD804E7DA7DFEDC6BE1FE9420CD7F30FAA085</t>
+  </si>
+  <si>
+    <t>C024F24EE42020B585EBFFA2D714FEABE6DB86EB399F383216A298127CDE9F50</t>
+  </si>
+  <si>
+    <t>FF9DCA8AECC63EFB7579C21B6D8EC6202DA99A96DAA0971F94374B62A8EECD05</t>
+  </si>
+  <si>
+    <t>FE743BF6615C16CAC68F1489D8A2278FD5E4D0D0D1E9D71CD73EFCB2C2867FAD</t>
+  </si>
+  <si>
+    <t>83F996C5CAA59E769D72E8BBE2CA3889988A442A2E58E58B5EFA9D7147A380BC</t>
+  </si>
+  <si>
+    <t>7FEBD98688C4830F308346A2D316FE7AC564CD41FC7481CA5E63198FB3C9A461</t>
+  </si>
+  <si>
+    <t>96EE871A28B49E2D73404F481891582213CE8ACFC64B2961281DFFDE88BD6B28</t>
+  </si>
+  <si>
+    <t>FBA6E2C56B5763DB64DBAD53C9DE9542A13CE98ED59E1C8079C983B283D03FC9</t>
+  </si>
+  <si>
+    <t>3E70F25D8ADE1197A9D52A6105AD8BF874ED26BD59EFFB7AF3044C1D2538337E</t>
+  </si>
+  <si>
+    <t>382E1AD864D1BC76F224C72653040D801656F82840C39CCD8E5222B3D680ECB7</t>
+  </si>
+  <si>
+    <t>B5890BD105E89F9F8BD01CC58D5037827890E5CB9CB999821A41BFB5BA9484CD</t>
+  </si>
+  <si>
+    <t>7CF8B2F5FFCCBDD59469E5421EC3657CDCBA84B931D5D58E7C7A44A38B04EFB7</t>
+  </si>
+  <si>
+    <t>E81ACED73E9ECBEDC1F9587D083082B7D334785BC666AB4E26B76BEF76982CFF</t>
+  </si>
+  <si>
+    <t>2F995B3EEB2CB47698168030C96342FB646E09988C2A20522B21A69F576A35B3</t>
+  </si>
+  <si>
+    <t>E0364ABBE0C4214D27DA3586F2EA089DE0453229ABE5D5733E60BC2D27B858ED</t>
+  </si>
+  <si>
+    <t>37625B4A678CFD7DE404411626CC421998A1881980CCD13DE636831F7E09AF5D</t>
+  </si>
+  <si>
+    <t>2E41E87B45DA427DF0EA7CA9D51289160617B30D118073A18B0CFB177272D2E9</t>
+  </si>
+  <si>
+    <t>6E04740025AA07E0D2447E5FF7960BCBC2A324DAED17591EE959BF6C20718A71</t>
+  </si>
+  <si>
+    <t>1B9A35C814BF3B3E3DFA9C6D19F8D8D7780F169D0CB4001CBC3A7CD20C3A12DF</t>
+  </si>
+  <si>
+    <t>9BD85F453F6B54A3C99AF89323AA045705B689465527349892A388C116FC722C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +334,20 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="3">
@@ -235,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -248,6 +410,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,8 +726,8 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,54 +744,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -638,28 +809,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="87.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -674,28 +847,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="85.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -710,28 +885,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="85.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -746,28 +923,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="87.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -780,14 +959,392 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="84.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="83.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="84.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="83" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="86.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="85.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -795,304 +1352,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1105,43 +1373,73 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="83.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1153,43 +1451,74 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="85.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1207,7 +1536,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1305,7 +1634,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1354,32 +1685,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1411,10 +1742,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1422,16 +1753,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1463,10 +1794,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1474,16 +1805,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1515,10 +1846,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1526,16 +1857,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1551,7 +1882,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,10 +1898,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1578,16 +1909,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1602,28 +1933,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="88.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1638,28 +1971,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="87.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
osmanbo add stage-3 B1-B2
</commit_message>
<xml_diff>
--- a/osmanbo/evidence.xlsx
+++ b/osmanbo/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osman\Desktop\gon_nft\osmanbo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9EA693-E3FA-4F37-9162-872B6D5B2555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3B02DC-FBE3-4403-8867-4A264BBCB400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3345" yWindow="630" windowWidth="31740" windowHeight="13155" firstSheet="2" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16065" yWindow="390" windowWidth="20670" windowHeight="13155" firstSheet="11" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="90">
   <si>
     <t>TxHash</t>
   </si>
@@ -315,6 +315,18 @@
   </si>
   <si>
     <t>9BD85F453F6B54A3C99AF89323AA045705B689465527349892A388C116FC722C</t>
+  </si>
+  <si>
+    <t>B59D759CFC2B3C2467393581B0279F6D59B7A5E072B382822337C16AC1EF6355</t>
+  </si>
+  <si>
+    <t>A9FBE0099069CFA335599822C53EA91212E0E282AC286CB91FB58C25E45C3C53</t>
+  </si>
+  <si>
+    <t>9A8E8DD23F9B39130FE14E70BC9A85398D76DFDAAC2E5D5969B4188D305E3AC2</t>
+  </si>
+  <si>
+    <t>34F863AD81C8009FFFB0FD67EB2464852BB887EB3C64862A56A0F37099FAB5E4</t>
   </si>
 </sst>
 </file>
@@ -397,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -419,6 +431,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,8 +741,8 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,7 +1468,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -1532,11 +1547,13 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="40" style="3" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="100.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1546,12 +1563,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" s="11" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1566,11 +1583,13 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="85.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1580,12 +1599,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
osmanbo update stage-2 evidence A16
</commit_message>
<xml_diff>
--- a/osmanbo/evidence.xlsx
+++ b/osmanbo/evidence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osman\Desktop\gon_nft\osmanbo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osman\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3B02DC-FBE3-4403-8867-4A264BBCB400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B7E649-65E6-4387-A299-991FF5299841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16065" yWindow="390" windowWidth="20670" windowHeight="13155" firstSheet="11" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22635" yWindow="2685" windowWidth="28875" windowHeight="15675" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -48,8 +48,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -57,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
   <si>
     <t>TxHash</t>
   </si>
@@ -248,15 +246,6 @@
     <t>8F4582EC69F88142E98B2B72B9F5AB6159D03FB5B5793FF2C5E520E0FDCE3DDB</t>
   </si>
   <si>
-    <t>9BC0FE63EED6B1AF48CA5FCFF3E667C07561363198162712A11667D89D617AD9</t>
-  </si>
-  <si>
-    <t>F9728568C28B7DD502CD792C198A1CB9027A1B69F028A7B5750F1CF47BD3BE8A</t>
-  </si>
-  <si>
-    <t>603AAF1F655C371D365381E6D1F1E1339B0F6C8BB26A63D7CC44FFBBA7BAD5EB</t>
-  </si>
-  <si>
     <t>82A9621DE4D2732FE7ACED1FCB0DD804E7DA7DFEDC6BE1FE9420CD7F30FAA085</t>
   </si>
   <si>
@@ -327,6 +316,18 @@
   </si>
   <si>
     <t>34F863AD81C8009FFFB0FD67EB2464852BB887EB3C64862A56A0F37099FAB5E4</t>
+  </si>
+  <si>
+    <t>582DF17E68D1561E5B664F87994D96097E637E12B1F54D8556C0934B2F44F2E6</t>
+  </si>
+  <si>
+    <t>B71433DD21E1D7BE6CDE93E2AEFF0E4168539114A8BBA0DEA3FE4A0FE54F8CF5</t>
+  </si>
+  <si>
+    <t>E30981FF790918FA5627E9BED2E2EFE680F9B389897556C1FF7C81EF19F139DD</t>
+  </si>
+  <si>
+    <t>18E7FFCD36CD0D22B69ED4FB95BCCB48537F1BE4AAF49CA9455A6959FB522414</t>
   </si>
 </sst>
 </file>
@@ -409,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -417,20 +418,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -739,7 +737,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -747,14 +745,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -784,33 +782,30 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -830,8 +825,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="87.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -868,8 +863,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="85.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="85.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -906,8 +901,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="85.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="85.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -944,8 +939,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="87.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -974,7 +969,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -982,52 +977,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="84.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1047,47 +1039,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="83.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1110,47 +1102,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="84.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1166,58 +1158,59 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="83" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="83" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1234,47 +1227,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="86.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="86.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1296,48 +1289,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="85.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="85.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1359,7 +1352,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1371,10 +1364,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1396,63 +1389,63 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="83.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="B5" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1474,64 +1467,64 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="85.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="85.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="B5" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1553,7 +1546,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="100.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1563,12 +1556,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>87</v>
+      <c r="A3" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1583,13 +1576,13 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="85.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="85.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1599,12 +1592,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1623,7 +1616,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1659,7 +1652,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1695,8 +1688,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="3" customWidth="1"/>
+    <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1711,24 +1704,24 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1750,10 +1743,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1771,16 +1764,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1802,10 +1795,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1823,16 +1816,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1854,10 +1847,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="64.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1878,7 +1871,7 @@
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1906,10 +1899,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="84.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1930,13 +1923,13 @@
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1958,8 +1951,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1996,8 +1989,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="87.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
osmanbo add evidence stage-3 round-4 (B5-B6-B7)
</commit_message>
<xml_diff>
--- a/osmanbo/evidence.xlsx
+++ b/osmanbo/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osman\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osman\Desktop\osmanbo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B7E649-65E6-4387-A299-991FF5299841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{417D04B0-DCDA-4541-86F7-463E807DE539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22635" yWindow="2685" windowWidth="28875" windowHeight="15675" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4395" yWindow="3630" windowWidth="28875" windowHeight="15660" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,17 +56,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="94">
   <si>
     <t>TxHash</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
@@ -246,6 +241,15 @@
     <t>8F4582EC69F88142E98B2B72B9F5AB6159D03FB5B5793FF2C5E520E0FDCE3DDB</t>
   </si>
   <si>
+    <t>9BC0FE63EED6B1AF48CA5FCFF3E667C07561363198162712A11667D89D617AD9</t>
+  </si>
+  <si>
+    <t>F9728568C28B7DD502CD792C198A1CB9027A1B69F028A7B5750F1CF47BD3BE8A</t>
+  </si>
+  <si>
+    <t>603AAF1F655C371D365381E6D1F1E1339B0F6C8BB26A63D7CC44FFBBA7BAD5EB</t>
+  </si>
+  <si>
     <t>82A9621DE4D2732FE7ACED1FCB0DD804E7DA7DFEDC6BE1FE9420CD7F30FAA085</t>
   </si>
   <si>
@@ -318,23 +322,29 @@
     <t>34F863AD81C8009FFFB0FD67EB2464852BB887EB3C64862A56A0F37099FAB5E4</t>
   </si>
   <si>
-    <t>582DF17E68D1561E5B664F87994D96097E637E12B1F54D8556C0934B2F44F2E6</t>
-  </si>
-  <si>
-    <t>B71433DD21E1D7BE6CDE93E2AEFF0E4168539114A8BBA0DEA3FE4A0FE54F8CF5</t>
-  </si>
-  <si>
-    <t>E30981FF790918FA5627E9BED2E2EFE680F9B389897556C1FF7C81EF19F139DD</t>
-  </si>
-  <si>
-    <t>18E7FFCD36CD0D22B69ED4FB95BCCB48537F1BE4AAF49CA9455A6959FB522414</t>
+    <t>697E67A6EA2D5B2713BA9652C2B65CB3F4A035EA4AD6CCA7CF273431BB9383D3</t>
+  </si>
+  <si>
+    <t>F748D6F75397C03E8AD8FEC4BB00E4CF11FF7185D0D0C5FA33A92CF1E924672B</t>
+  </si>
+  <si>
+    <t>187C1BAE5E2E6A4228556F57100FC2F417213BDA3E201A7552694B076C33593C</t>
+  </si>
+  <si>
+    <t>CEEA88F15B15DF44016EBCC28B1384ABC124794CE6FA20A69CF348341E3BF0A4</t>
+  </si>
+  <si>
+    <t>551803E9386E70EEDF6C55998D20DF647E2A55BAF9AEFF0C3F83926911CBF8D5</t>
+  </si>
+  <si>
+    <t>CCBACBF243E313D87E229E0B1F591E67BDCC1F20BAD74407AE3B346CFA97CC54</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,8 +372,14 @@
       <family val="2"/>
       <charset val="162"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,6 +389,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFC6C6C6"/>
       </patternFill>
     </fill>
   </fills>
@@ -410,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -431,6 +453,15 @@
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,54 +788,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -831,10 +862,48 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="85.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -850,29 +919,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="85.42578125" bestFit="1" customWidth="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="85.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -888,29 +957,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="85.7109375" bestFit="1" customWidth="1"/>
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="87.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -926,44 +995,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="87.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
@@ -986,39 +1017,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1048,39 +1079,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1111,31 +1142,93 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="83" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="B4" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1143,28 +1236,28 @@
         <v>62</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="83" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="86.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1173,62 +1266,161 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>89</v>
+        <v>66</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="85.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="86.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="83.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1236,60 +1428,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="85.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="85.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="5"/>
   </cols>
@@ -1299,233 +1507,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>70</v>
+      <c r="A5" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="83.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="85.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1556,12 +1586,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1592,12 +1622,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1612,11 +1642,13 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="89.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1626,12 +1658,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1647,12 +1679,12 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="82.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1662,12 +1694,45 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{602B0C21-A131-4B17-9A89-3AC6958EB5B0}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="83.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1697,32 +1762,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1754,27 +1819,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1806,27 +1871,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1858,27 +1923,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1910,27 +1975,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1957,10 +2022,48 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="87.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1974,42 +2077,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="87.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>